<commit_message>
1. Implemented test cases for roundtrip test.
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/Flight_Search_Regression.xlsx
+++ b/src/main/resources/testdata/Flight_Search_Regression.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Automation\Wego_FlightSearch_Automation\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49295FFF-AEAC-4868-B449-2619361F48C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD792BB-1A29-46B3-A81D-3254F2219ACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
   <si>
     <t>Test Name</t>
   </si>
@@ -91,6 +91,30 @@
   </si>
   <si>
     <t>2 January 2023</t>
+  </si>
+  <si>
+    <t>roundTripFlightSearch</t>
+  </si>
+  <si>
+    <t>28 December 2022</t>
+  </si>
+  <si>
+    <t>Round-trip</t>
+  </si>
+  <si>
+    <t>22 January 2023</t>
+  </si>
+  <si>
+    <t>28 March 2023</t>
+  </si>
+  <si>
+    <t>Kolkata</t>
+  </si>
+  <si>
+    <t>12 January 2023</t>
+  </si>
+  <si>
+    <t>13 January 2023</t>
   </si>
 </sst>
 </file>
@@ -183,11 +207,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
@@ -472,7 +497,7 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,43 +645,98 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2">
+        <v>2</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="2">
+        <v>3</v>
+      </c>
+      <c r="G6" s="2">
+        <v>2</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
+      <c r="B7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="2">
+        <v>5</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
@@ -669,7 +749,6 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>

</xml_diff>

<commit_message>
1. Changes test data
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/Flight_Search_Regression.xlsx
+++ b/src/main/resources/testdata/Flight_Search_Regression.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Automation\Wego_FlightSearch_Automation\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD792BB-1A29-46B3-A81D-3254F2219ACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E161A7-9C4C-414C-840C-71B000C85961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -93,9 +93,6 @@
     <t>2 January 2023</t>
   </si>
   <si>
-    <t>roundTripFlightSearch</t>
-  </si>
-  <si>
     <t>28 December 2022</t>
   </si>
   <si>
@@ -115,6 +112,9 @@
   </si>
   <si>
     <t>13 January 2023</t>
+  </si>
+  <si>
+    <t>RoundTripFlightSearch</t>
   </si>
 </sst>
 </file>
@@ -646,7 +646,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>17</v>
@@ -658,7 +658,7 @@
         <v>19</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="2">
         <v>1</v>
@@ -673,7 +673,7 @@
         <v>13</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -681,13 +681,13 @@
         <v>17</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="F6" s="2">
         <v>3</v>
@@ -702,10 +702,10 @@
         <v>13</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -717,10 +717,10 @@
         <v>10</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="F7" s="2">
         <v>5</v>
@@ -735,7 +735,7 @@
         <v>13</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>